<commit_message>
Split out strobe circuit into its own module
</commit_message>
<xml_diff>
--- a/electrical/TurntableMain-BOM.xlsx
+++ b/electrical/TurntableMain-BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11194B2-6E79-4A88-BB14-7C092E37D652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5678F6-1069-460C-9E56-7346A3C1D5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="112">
   <si>
     <t>A1</t>
   </si>
@@ -279,12 +279,6 @@
     <t>Take from MX1508 PCB</t>
   </si>
   <si>
-    <t>J1, J21</t>
-  </si>
-  <si>
-    <t>J9, J12, J13, J14, J15, J16, J17, J20, J22, J23</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
@@ -303,18 +297,6 @@
     <t>J19</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>????</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
@@ -360,25 +342,31 @@
     <t>Price estimates are as of 3 Sept. 2022</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D17, D18, D19</t>
-  </si>
-  <si>
-    <t>Q1, Q2, Q3, Q4, Q5</t>
-  </si>
-  <si>
     <t>R5, R7, R8, R9, R11, R12, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R42, R43</t>
   </si>
   <si>
-    <t>R6, R10, R13, R14, R15, R41, R44</t>
-  </si>
-  <si>
-    <t>RL1, RL2, RL3, RL4</t>
-  </si>
-  <si>
     <t>J3, J4</t>
   </si>
   <si>
-    <t>J5, J6, J7, J8, J18, J24, J25, J26, J27</t>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D13, D14, D15, D17, D18, D19</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q4, Q5</t>
+  </si>
+  <si>
+    <t>R10, R13, R14, R15, R44</t>
+  </si>
+  <si>
+    <t>RL1, RL3, RL4</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J9, J12, J13, J14, J15, J16, J17, J22, J23</t>
+  </si>
+  <si>
+    <t>J5, J6, J7, J8, J18, J24, J25, J26, J27, J39</t>
   </si>
 </sst>
 </file>
@@ -1020,8 +1008,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J31" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
@@ -1335,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1400,7 @@
         <v>10.38</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1529,7 +1517,7 @@
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -1546,10 +1534,11 @@
         <v>27</v>
       </c>
       <c r="H7" s="5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="6">
-        <v>1.89</v>
+        <f>0.2408*17</f>
+        <v>4.0935999999999995</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -1581,7 +1570,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
@@ -1596,19 +1585,19 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" s="6">
-        <v>0.82</v>
+        <v>0.41</v>
       </c>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5" t="s">
@@ -1620,7 +1609,7 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>67</v>
@@ -1629,7 +1618,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>33</v>
@@ -1655,7 +1644,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>64</v>
@@ -1670,7 +1659,7 @@
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>67</v>
@@ -1681,7 +1670,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>65</v>
@@ -1705,7 +1694,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>34</v>
@@ -1729,7 +1718,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>66</v>
@@ -1753,7 +1742,7 @@
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>35</v>
@@ -1777,7 +1766,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>5</v>
@@ -1794,383 +1783,332 @@
         <v>36</v>
       </c>
       <c r="H17" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I17" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="5">
         <v>1</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="H19" s="5">
-        <v>1</v>
-      </c>
-      <c r="I19" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="I19" s="6">
+        <v>2.57</v>
+      </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="5">
+        <v>5</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5" t="s">
+      <c r="E21" s="4"/>
+      <c r="F21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5">
+      <c r="G21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="5">
+        <v>2</v>
+      </c>
+      <c r="I21" s="6">
+        <v>3.93</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5">
         <v>1</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="5">
-        <v>18</v>
-      </c>
       <c r="I22" s="6">
-        <v>2.57</v>
+        <v>0.79</v>
       </c>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>29</v>
+      <c r="G23" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="H23" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I23" s="6">
-        <v>0.77</v>
+        <v>1.64</v>
       </c>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="E24" s="5"/>
       <c r="F24" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>98</v>
+        <v>22</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="H24" s="5">
-        <v>4</v>
-      </c>
-      <c r="I24" s="6">
-        <v>5.24</v>
-      </c>
-      <c r="J24" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5">
         <v>1</v>
       </c>
-      <c r="I25" s="6">
-        <v>0.79</v>
-      </c>
-      <c r="J25" s="5"/>
+      <c r="I25" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="D26" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="F26" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="H26" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I26" s="6">
-        <v>1.64</v>
+        <v>9.4</v>
       </c>
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="5" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="H27" s="5">
-        <v>2</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I27" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="5">
-        <v>1</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A28" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="12">
+        <f>SUM(H2:H27)</f>
         <v>101</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H29" s="5">
-        <v>2</v>
-      </c>
-      <c r="I29" s="6">
-        <v>9.4</v>
-      </c>
-      <c r="J29" s="5"/>
+      <c r="I28" s="13">
+        <f>SUM(I2:I27)</f>
+        <v>42.913600000000002</v>
+      </c>
+      <c r="J28" s="12"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H30" s="5">
-        <v>1</v>
-      </c>
-      <c r="I30" s="6">
-        <v>0.49</v>
-      </c>
-      <c r="J30" s="5"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="12">
-        <f>SUM(H2:H30)</f>
-        <v>111</v>
-      </c>
-      <c r="I31" s="13">
-        <f>SUM(I2:I30)</f>
-        <v>43.650000000000006</v>
-      </c>
-      <c r="J31" s="12"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -2222,11 +2160,6 @@
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-    </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
@@ -2237,20 +2170,20 @@
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
@@ -2282,6 +2215,11 @@
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
     </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+    </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
@@ -2341,21 +2279,6 @@
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish PCB v5 BOM
</commit_message>
<xml_diff>
--- a/electrical/TurntableMain-BOM.xlsx
+++ b/electrical/TurntableMain-BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5678F6-1069-460C-9E56-7346A3C1D5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA70245-46AE-49DB-A5E9-7BA49B45978B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="120">
   <si>
     <t>A1</t>
   </si>
@@ -42,15 +42,9 @@
     <t>Ceramic Capacitor</t>
   </si>
   <si>
-    <t>Rectifier Diode</t>
-  </si>
-  <si>
     <t>Screw terminal - 2 pins</t>
   </si>
   <si>
-    <t>Basic FET P-Channel</t>
-  </si>
-  <si>
     <t>ULN2003A</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>Price Est.</t>
   </si>
   <si>
-    <t>TIP120</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -114,9 +105,6 @@
     <t>Value(s)</t>
   </si>
   <si>
-    <t>300 mil</t>
-  </si>
-  <si>
     <t>C0603C104K4NACAUTO</t>
   </si>
   <si>
@@ -126,9 +114,6 @@
     <t>0.1µF; 35V</t>
   </si>
   <si>
-    <t>1N4007</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -210,9 +195,6 @@
     <t>KF2510 3-pin</t>
   </si>
   <si>
-    <t>74AUC1G08</t>
-  </si>
-  <si>
     <t>5v; 3a</t>
   </si>
   <si>
@@ -252,27 +234,12 @@
     <t>BHR-06-VUA</t>
   </si>
   <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>C1, C2</t>
-  </si>
-  <si>
     <t>100µF; 16v</t>
   </si>
   <si>
     <t>n/a</t>
   </si>
   <si>
-    <t>C4, C13</t>
-  </si>
-  <si>
-    <t>C3, C5, C6, C7, C8, C9, C10, C11, C12</t>
-  </si>
-  <si>
-    <t>D16</t>
-  </si>
-  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -288,36 +255,12 @@
     <t>Developer recommends using 30-pin DIP socket. DE37566 pins may need to be used.</t>
   </si>
   <si>
-    <t>J28</t>
-  </si>
-  <si>
-    <t>J10, J11</t>
-  </si>
-  <si>
-    <t>J19</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
     <t>220Ω</t>
   </si>
   <si>
-    <t>Relay</t>
-  </si>
-  <si>
-    <t>J104D2C5VDC.20S</t>
-  </si>
-  <si>
-    <t>DPDT (2 Form C)</t>
-  </si>
-  <si>
-    <t>U8, U9, U10, U11</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
     <t>U1, U6</t>
   </si>
   <si>
@@ -342,31 +285,112 @@
     <t>Price estimates are as of 3 Sept. 2022</t>
   </si>
   <si>
-    <t>R5, R7, R8, R9, R11, R12, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R42, R43</t>
-  </si>
-  <si>
     <t>J3, J4</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D13, D14, D15, D17, D18, D19</t>
-  </si>
-  <si>
-    <t>Q1, Q2, Q4, Q5</t>
-  </si>
-  <si>
-    <t>R10, R13, R14, R15, R44</t>
-  </si>
-  <si>
-    <t>RL1, RL3, RL4</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>J9, J12, J13, J14, J15, J16, J17, J22, J23</t>
-  </si>
-  <si>
-    <t>J5, J6, J7, J8, J18, J24, J25, J26, J27, J39</t>
+    <t>C2, C3</t>
+  </si>
+  <si>
+    <t>C1, C5, C6, C7, C8, C9, C10, C12, C13, C14, C15, C17, C19, C21, C22, C23, C24</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C4, C11</t>
+  </si>
+  <si>
+    <t>C16, C18</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>generic male header - 1 pin (1 row)</t>
+  </si>
+  <si>
+    <t>J5, J9, J10, J11, J13, J14, J15, J17</t>
+  </si>
+  <si>
+    <t>J7, J8</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>male header 5 pin (1 row)</t>
+  </si>
+  <si>
+    <t>KF2510 5-pin</t>
+  </si>
+  <si>
+    <t>J16, J18, J19</t>
+  </si>
+  <si>
+    <t>Comes in lot listed on main parts list.</t>
+  </si>
+  <si>
+    <t>DE37566</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>J20</t>
+  </si>
+  <si>
+    <t>J21</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R8, R9, R10, R11, R12, R13, R14, R15, R16</t>
+  </si>
+  <si>
+    <t>R5, R6, R7</t>
+  </si>
+  <si>
+    <t>U7, U10, U11, U12, U13, U14</t>
+  </si>
+  <si>
+    <t>"Or" gate</t>
+  </si>
+  <si>
+    <t>5v</t>
+  </si>
+  <si>
+    <t>MC74VHC1G32DTT1G</t>
+  </si>
+  <si>
+    <t>U8, U9</t>
+  </si>
+  <si>
+    <t>U15, U16, U17, U18</t>
+  </si>
+  <si>
+    <t>06033C473KAT2A</t>
+  </si>
+  <si>
+    <t>47nF; 25v</t>
+  </si>
+  <si>
+    <t>SN74AUC1G08DCKR</t>
+  </si>
+  <si>
+    <t>B330AF-13</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>30v; 3a</t>
+  </si>
+  <si>
+    <t>DO-221AC, SMA</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1032,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J30" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
@@ -1323,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,34 +1369,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1380,18 +1404,18 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
@@ -1400,84 +1424,84 @@
         <v>10.38</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H3" s="5">
-        <v>2</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>81</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1.48</v>
+      </c>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>29</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G4" s="4"/>
       <c r="H4" s="5">
-        <v>9</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1.08</v>
-      </c>
-      <c r="J4" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
@@ -1489,23 +1513,23 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H6" s="5">
         <v>2</v>
@@ -1515,595 +1539,650 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="D7" s="5" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="H7" s="5">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I7" s="6">
-        <f>0.2408*17</f>
-        <v>4.0935999999999995</v>
+        <v>0.2</v>
       </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="5">
         <v>1</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H9" s="5">
         <v>1</v>
       </c>
-      <c r="I9" s="6">
-        <v>0.41</v>
+      <c r="I9" s="9">
+        <v>0.44</v>
       </c>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7"/>
       <c r="F10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="5">
-        <v>10</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>67</v>
+        <v>1</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.41</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>72</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E11" s="7"/>
       <c r="F11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="G11" s="4"/>
       <c r="H11" s="5">
-        <v>2</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0.96</v>
-      </c>
-      <c r="J11" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="F12" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5">
-        <v>9</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>68</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.96</v>
+      </c>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="5" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5">
         <v>1</v>
       </c>
-      <c r="I14" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="J14" s="5"/>
+      <c r="I14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
         <v>2</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="8"/>
+        <v>72</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="5">
-        <v>1</v>
-      </c>
-      <c r="I16" s="9">
-        <v>0.73</v>
-      </c>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C17" s="8"/>
       <c r="D17" s="5" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>36</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G17" s="5"/>
       <c r="H17" s="5">
-        <v>4</v>
-      </c>
-      <c r="I17" s="6">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0.73</v>
       </c>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="G18" s="5"/>
       <c r="H18" s="5">
         <v>1</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>29</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G19" s="5"/>
       <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="6">
-        <v>2.57</v>
-      </c>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="G20" s="8" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="H20" s="5">
-        <v>5</v>
-      </c>
-      <c r="I20" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5" t="s">
-        <v>91</v>
+        <v>27</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="H21" s="5">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I21" s="6">
-        <v>3.93</v>
+        <v>1.68</v>
       </c>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="4"/>
       <c r="F22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H22" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I22" s="6">
-        <v>0.79</v>
+        <v>0.33</v>
       </c>
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="D23" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="F23" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="H23" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I23" s="6">
-        <v>1.64</v>
+        <v>9.4</v>
       </c>
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H24" s="5">
         <v>2</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="5" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5">
         <v>1</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="G26" s="4"/>
       <c r="H26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" s="6">
-        <v>9.4</v>
+        <v>0.79</v>
       </c>
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="D27" s="5" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H27" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I27" s="6">
-        <v>0.49</v>
+        <v>2.88</v>
       </c>
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="12">
-        <f>SUM(H2:H27)</f>
-        <v>101</v>
-      </c>
-      <c r="I28" s="13">
-        <f>SUM(I2:I27)</f>
-        <v>42.913600000000002</v>
-      </c>
-      <c r="J28" s="12"/>
+      <c r="A28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="5">
+        <v>2</v>
+      </c>
+      <c r="I28" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" s="5">
+        <v>4</v>
+      </c>
+      <c r="I29" s="6">
+        <v>1.64</v>
+      </c>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="A30" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="12">
+        <f>SUM(H2:H29)</f>
+        <v>82</v>
+      </c>
+      <c r="I30" s="13">
+        <f>SUM(I2:I29)</f>
+        <v>34.19</v>
+      </c>
+      <c r="J30" s="12"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>102</v>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -2160,61 +2239,61 @@
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+    </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+    </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-    </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
@@ -2279,6 +2358,16 @@
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update main BOM to account for PCB changes
</commit_message>
<xml_diff>
--- a/electrical/TurntableMain-BOM.xlsx
+++ b/electrical/TurntableMain-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA70245-46AE-49DB-A5E9-7BA49B45978B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40C3B6C-A375-48C9-A6E1-7937DE14D408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="285" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -285,9 +285,6 @@
     <t>Price estimates are as of 3 Sept. 2022</t>
   </si>
   <si>
-    <t>J3, J4</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -315,9 +312,6 @@
     <t>generic male header - 1 pin (1 row)</t>
   </si>
   <si>
-    <t>J5, J9, J10, J11, J13, J14, J15, J17</t>
-  </si>
-  <si>
     <t>J7, J8</t>
   </si>
   <si>
@@ -391,6 +385,12 @@
   </si>
   <si>
     <t>DO-221AC, SMA</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J3, J5, J9, J10, J11, J13, J14, J15, J17</t>
   </si>
 </sst>
 </file>
@@ -1339,7 +1339,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1349,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="3" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>2</v>
@@ -1541,16 +1541,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
@@ -1569,7 +1569,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>69</v>
@@ -1595,23 +1595,23 @@
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H9" s="5">
         <v>1</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
@@ -1650,11 +1650,11 @@
         <v>71</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="5" t="s">
@@ -1668,12 +1668,12 @@
         <v>61</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>28</v>
@@ -1690,16 +1690,17 @@
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="6">
-        <v>0.96</v>
+        <f>0.96/2</f>
+        <v>0.48</v>
       </c>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>58</v>
@@ -1714,7 +1715,7 @@
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>61</v>
@@ -1725,14 +1726,14 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
@@ -1751,7 +1752,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>60</v>
@@ -1772,12 +1773,12 @@
         <v>61</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>72</v>
@@ -1803,7 +1804,7 @@
     </row>
     <row r="17" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>30</v>
@@ -1827,7 +1828,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>59</v>
@@ -1853,7 +1854,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>29</v>
@@ -1907,7 +1908,7 @@
     </row>
     <row r="21" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>27</v>
@@ -1935,7 +1936,7 @@
     </row>
     <row r="22" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>27</v>
@@ -2071,16 +2072,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
@@ -2099,14 +2100,14 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="s">
@@ -2125,7 +2126,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>64</v>
@@ -2165,7 +2166,7 @@
       </c>
       <c r="I30" s="13">
         <f>SUM(I2:I29)</f>
-        <v>34.19</v>
+        <v>33.71</v>
       </c>
       <c r="J30" s="12"/>
     </row>

</xml_diff>